<commit_message>
Add your test cases to excel
</commit_message>
<xml_diff>
--- a/src/test/resources/nopCommerce_FrontEnd_TestCases.xlsx
+++ b/src/test/resources/nopCommerce_FrontEnd_TestCases.xlsx
@@ -5,15 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharmin Zaman\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharmin Zaman\IdeaProjects\nopCommerce\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52725F91-B42B-46B3-90EC-ADEA5F0839E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB2656D-B895-4FA9-96D7-AA63753FB65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5BE317AF-6064-4EB0-BD7F-9D2C2ECF4852}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{5BE317AF-6064-4EB0-BD7F-9D2C2ECF4852}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="Sharmin" sheetId="1" r:id="rId1"/>
+    <sheet name="Nouredine" sheetId="2" r:id="rId2"/>
+    <sheet name="Khalil" sheetId="3" r:id="rId3"/>
+    <sheet name="Mehnaz" sheetId="4" r:id="rId4"/>
+    <sheet name="Malek" sheetId="5" r:id="rId5"/>
+    <sheet name="Madjid" sheetId="6" r:id="rId6"/>
+    <sheet name="Sabrina" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="90">
   <si>
     <t>Test Case</t>
   </si>
@@ -548,6 +554,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -564,15 +579,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -891,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA38DB8C-7CA1-4DCD-A03A-DCF703454A47}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -929,10 +935,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="24" t="s">
         <v>84</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -948,8 +954,8 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="25"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="7" t="s">
         <v>21</v>
       </c>
@@ -962,8 +968,8 @@
       <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="25"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="7" t="s">
         <v>24</v>
       </c>
@@ -976,8 +982,8 @@
       <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="25"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="8" t="s">
         <v>25</v>
       </c>
@@ -990,8 +996,8 @@
       <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="25"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="7" t="s">
         <v>27</v>
       </c>
@@ -1004,8 +1010,8 @@
       <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="25"/>
-      <c r="B7" s="22"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="7" t="s">
         <v>74</v>
       </c>
@@ -1018,8 +1024,8 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="25"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="8" t="s">
         <v>30</v>
       </c>
@@ -1032,8 +1038,8 @@
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="25"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="7" t="s">
         <v>32</v>
       </c>
@@ -1044,8 +1050,8 @@
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="25"/>
-      <c r="B10" s="22"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="7" t="s">
         <v>33</v>
       </c>
@@ -1058,8 +1064,8 @@
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="25"/>
-      <c r="B11" s="22"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="7" t="s">
         <v>35</v>
       </c>
@@ -1072,8 +1078,8 @@
       <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="25"/>
-      <c r="B12" s="22"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="7" t="s">
         <v>37</v>
       </c>
@@ -1086,8 +1092,8 @@
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="25"/>
-      <c r="B13" s="22"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="7" t="s">
         <v>39</v>
       </c>
@@ -1100,8 +1106,8 @@
       <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="25"/>
-      <c r="B14" s="22"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="7" t="s">
         <v>49</v>
       </c>
@@ -1114,8 +1120,8 @@
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="25"/>
-      <c r="B15" s="22"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="7" t="s">
         <v>45</v>
       </c>
@@ -1128,8 +1134,8 @@
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="25"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="7" t="s">
         <v>48</v>
       </c>
@@ -1142,8 +1148,8 @@
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="25"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="7" t="s">
         <v>51</v>
       </c>
@@ -1156,8 +1162,8 @@
       <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="25"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="7" t="s">
         <v>54</v>
       </c>
@@ -1170,8 +1176,8 @@
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="25"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="7" t="s">
         <v>60</v>
       </c>
@@ -1184,8 +1190,8 @@
       <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="25"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="7" t="s">
         <v>56</v>
       </c>
@@ -1198,8 +1204,8 @@
       <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="25"/>
-      <c r="B21" s="22"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="7" t="s">
         <v>57</v>
       </c>
@@ -1212,8 +1218,8 @@
       <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A22" s="25"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="11" t="s">
         <v>65</v>
       </c>
@@ -1226,8 +1232,8 @@
       <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A23" s="25"/>
-      <c r="B23" s="22"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="25"/>
       <c r="C23" s="11" t="s">
         <v>64</v>
       </c>
@@ -1240,8 +1246,8 @@
       <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="25"/>
-      <c r="B24" s="22"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="11" t="s">
         <v>66</v>
       </c>
@@ -1254,8 +1260,8 @@
       <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A25" s="25"/>
-      <c r="B25" s="22"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="11" t="s">
         <v>67</v>
       </c>
@@ -1266,8 +1272,8 @@
       <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="25"/>
-      <c r="B26" s="22"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="12" t="s">
         <v>68</v>
       </c>
@@ -1280,8 +1286,8 @@
       <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="25"/>
-      <c r="B27" s="22"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="25"/>
       <c r="C27" s="12" t="s">
         <v>69</v>
       </c>
@@ -1292,8 +1298,8 @@
       <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="26"/>
-      <c r="B28" s="23"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="13" t="s">
         <v>75</v>
       </c>
@@ -1303,10 +1309,10 @@
       <c r="G28" s="17"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="21" t="s">
         <v>83</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -1322,8 +1328,8 @@
       <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="25"/>
-      <c r="B30" s="28"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="8" t="s">
         <v>21</v>
       </c>
@@ -1336,8 +1342,8 @@
       <c r="G30" s="9"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="25"/>
-      <c r="B31" s="28"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="22"/>
       <c r="C31" s="7" t="s">
         <v>24</v>
       </c>
@@ -1350,8 +1356,8 @@
       <c r="G31" s="9"/>
     </row>
     <row r="32" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="25"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="22"/>
       <c r="C32" s="8" t="s">
         <v>25</v>
       </c>
@@ -1364,8 +1370,8 @@
       <c r="G32" s="9"/>
     </row>
     <row r="33" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="25"/>
-      <c r="B33" s="28"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="22"/>
       <c r="C33" s="7" t="s">
         <v>79</v>
       </c>
@@ -1378,8 +1384,8 @@
       <c r="G33" s="9"/>
     </row>
     <row r="34" spans="1:7" ht="40" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="26"/>
-      <c r="B34" s="29"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="14" t="s">
         <v>81</v>
       </c>
@@ -1396,7 +1402,7 @@
       <c r="A35" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="21" t="s">
         <v>89</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -1413,7 +1419,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="19"/>
-      <c r="B36" s="28"/>
+      <c r="B36" s="22"/>
       <c r="C36" s="7" t="s">
         <v>21</v>
       </c>
@@ -1427,7 +1433,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="19"/>
-      <c r="B37" s="28"/>
+      <c r="B37" s="22"/>
       <c r="C37" s="7" t="s">
         <v>22</v>
       </c>
@@ -1441,7 +1447,7 @@
     </row>
     <row r="38" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A38" s="19"/>
-      <c r="B38" s="28"/>
+      <c r="B38" s="22"/>
       <c r="C38" s="7" t="s">
         <v>13</v>
       </c>
@@ -1455,7 +1461,7 @@
     </row>
     <row r="39" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A39" s="19"/>
-      <c r="B39" s="28"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="7" t="s">
         <v>12</v>
       </c>
@@ -1469,7 +1475,7 @@
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="19"/>
-      <c r="B40" s="28"/>
+      <c r="B40" s="22"/>
       <c r="C40" s="7" t="s">
         <v>87</v>
       </c>
@@ -1485,7 +1491,7 @@
       <c r="A41" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="21" t="s">
         <v>86</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -1502,7 +1508,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="19"/>
-      <c r="B42" s="28"/>
+      <c r="B42" s="22"/>
       <c r="C42" s="7" t="s">
         <v>21</v>
       </c>
@@ -1516,7 +1522,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="19"/>
-      <c r="B43" s="28"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="7" t="s">
         <v>22</v>
       </c>
@@ -1530,7 +1536,7 @@
     </row>
     <row r="44" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A44" s="19"/>
-      <c r="B44" s="28"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="7" t="s">
         <v>13</v>
       </c>
@@ -1544,7 +1550,7 @@
     </row>
     <row r="45" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A45" s="19"/>
-      <c r="B45" s="28"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="7" t="s">
         <v>12</v>
       </c>
@@ -1558,7 +1564,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="19"/>
-      <c r="B46" s="28"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="7" t="s">
         <v>87</v>
       </c>
@@ -1572,7 +1578,7 @@
     </row>
     <row r="47" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A47" s="19"/>
-      <c r="B47" s="28"/>
+      <c r="B47" s="22"/>
       <c r="C47" s="8" t="s">
         <v>15</v>
       </c>
@@ -1586,7 +1592,7 @@
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="20"/>
-      <c r="B48" s="29"/>
+      <c r="B48" s="23"/>
       <c r="C48" s="15" t="s">
         <v>17</v>
       </c>
@@ -1615,4 +1621,267 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3124BC80-FB1E-47DD-931D-D7932A9376F3}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2924D075-7A2C-4988-BF88-36EAFC14652B}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7359425C-0B41-4C71-89B4-A9A79147A9A2}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A088F9E1-D822-471E-B051-AB9AC78DDB3B}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5B31F8-1D6C-4FE9-8196-2D698DAA4DDA}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A569904C-E53A-44CB-AA02-0DBE012274D9}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Check resgistereduser test case
</commit_message>
<xml_diff>
--- a/src/test/resources/nopCommerce_FrontEnd_TestCases.xlsx
+++ b/src/test/resources/nopCommerce_FrontEnd_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharmin Zaman\IdeaProjects\nopCommerce\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB2656D-B895-4FA9-96D7-AA63753FB65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF3A756-6965-4495-83FB-AF48B016AE31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{5BE317AF-6064-4EB0-BD7F-9D2C2ECF4852}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5BE317AF-6064-4EB0-BD7F-9D2C2ECF4852}"/>
   </bookViews>
   <sheets>
     <sheet name="Sharmin" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="114">
   <si>
     <t>Test Case</t>
   </si>
@@ -153,21 +153,12 @@
     <t>Enter first name</t>
   </si>
   <si>
-    <t>Sharmin</t>
-  </si>
-  <si>
     <t>Enter last name</t>
   </si>
   <si>
-    <t>Zaman</t>
-  </si>
-  <si>
     <t>Enter email</t>
   </si>
   <si>
-    <t>zamansharmin000@gmail.com</t>
-  </si>
-  <si>
     <t>Value entered appears on the firstname field</t>
   </si>
   <si>
@@ -201,18 +192,12 @@
     <t>Select state</t>
   </si>
   <si>
-    <t>New York</t>
-  </si>
-  <si>
     <t>Value appears in state field</t>
   </si>
   <si>
     <t>Enter city</t>
   </si>
   <si>
-    <t>Queens</t>
-  </si>
-  <si>
     <t>Enter zipcode</t>
   </si>
   <si>
@@ -232,9 +217,6 @@
   </si>
   <si>
     <t>Value entered appears on the phone number field</t>
-  </si>
-  <si>
-    <t>Shometheifjew</t>
   </si>
   <si>
     <t>Click Shipping Method continue button</t>
@@ -350,6 +332,96 @@
   </si>
   <si>
     <t>Test: Add to wishlist</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>Test: Register for an account</t>
+  </si>
+  <si>
+    <t>Click on Register</t>
+  </si>
+  <si>
+    <t>Naviagte to register page</t>
+  </si>
+  <si>
+    <t>Choose radio option button for gender</t>
+  </si>
+  <si>
+    <t>Radio button fills for chosen gender</t>
+  </si>
+  <si>
+    <t>First name appears in fields</t>
+  </si>
+  <si>
+    <t>Last name appears in fields</t>
+  </si>
+  <si>
+    <t>Click on day dropdown</t>
+  </si>
+  <si>
+    <t>Select day</t>
+  </si>
+  <si>
+    <t>Click on month dropdown</t>
+  </si>
+  <si>
+    <t>Select month</t>
+  </si>
+  <si>
+    <t>Click on year dropdown</t>
+  </si>
+  <si>
+    <t>Select year</t>
+  </si>
+  <si>
+    <t>Day dropdown selection appear</t>
+  </si>
+  <si>
+    <t>Month dropdown selection appear</t>
+  </si>
+  <si>
+    <t>Year dropdown selection appear</t>
+  </si>
+  <si>
+    <t>Day selected is in field</t>
+  </si>
+  <si>
+    <t>Month selected is in field</t>
+  </si>
+  <si>
+    <t>Year selected is in field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter email </t>
+  </si>
+  <si>
+    <t>Email appears in field</t>
+  </si>
+  <si>
+    <t>Enter password</t>
+  </si>
+  <si>
+    <t>Enter password in confirm password field</t>
+  </si>
+  <si>
+    <t>Password appears in field</t>
+  </si>
+  <si>
+    <t>Click register</t>
+  </si>
+  <si>
+    <t>msg - "Your registration completed"</t>
+  </si>
+  <si>
+    <t>Random generator</t>
+  </si>
+  <si>
+    <t>Random generator + @gmail.com</t>
+  </si>
+  <si>
+    <t>(718) + Random generator</t>
   </si>
 </sst>
 </file>
@@ -396,14 +468,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -413,6 +477,13 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -519,9 +590,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -534,14 +605,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -552,7 +622,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -580,6 +649,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -895,10 +978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA38DB8C-7CA1-4DCD-A03A-DCF703454A47}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -916,7 +999,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -935,11 +1018,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>84</v>
+      <c r="A2" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>78</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>8</v>
@@ -954,8 +1037,8 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="28"/>
-      <c r="B3" s="25"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="7" t="s">
         <v>21</v>
       </c>
@@ -968,8 +1051,8 @@
       <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="28"/>
-      <c r="B4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="7" t="s">
         <v>24</v>
       </c>
@@ -982,8 +1065,8 @@
       <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="28"/>
-      <c r="B5" s="25"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="8" t="s">
         <v>25</v>
       </c>
@@ -996,8 +1079,8 @@
       <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="28"/>
-      <c r="B6" s="25"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="7" t="s">
         <v>27</v>
       </c>
@@ -1010,10 +1093,10 @@
       <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="28"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>9</v>
@@ -1024,8 +1107,8 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="28"/>
-      <c r="B8" s="25"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="8" t="s">
         <v>30</v>
       </c>
@@ -1038,8 +1121,8 @@
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="28"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="7" t="s">
         <v>32</v>
       </c>
@@ -1050,8 +1133,8 @@
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="28"/>
-      <c r="B10" s="25"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="7" t="s">
         <v>33</v>
       </c>
@@ -1064,206 +1147,206 @@
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="28"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="26"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="D12" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="26"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="26"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="28"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="26"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="28"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="7" t="s">
+      <c r="E15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="26"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="26"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="28"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="28"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="8" t="s">
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="26"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="28"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="7" t="s">
+      <c r="D18" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="26"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="26"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D20" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="26"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="28"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="8" t="s">
+      <c r="D21" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+      <c r="A22" s="26"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+      <c r="A23" s="26"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="28"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="7" t="s">
+      <c r="D23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="26"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="28"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="7">
-        <v>12344</v>
-      </c>
-      <c r="E20" s="8" t="s">
+      <c r="D24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.35">
+      <c r="A25" s="26"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="28"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="10">
-        <v>234567654321</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" s="9"/>
-    </row>
-    <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A22" s="28"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A23" s="28"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.35">
-      <c r="A25" s="28"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="11" t="s">
-        <v>67</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>9</v>
@@ -1272,24 +1355,24 @@
       <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="12" t="s">
-        <v>68</v>
+      <c r="A26" s="26"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="28"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="12" t="s">
-        <v>69</v>
+      <c r="A27" s="26"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>9</v>
@@ -1298,22 +1381,22 @@
       <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="29"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="17"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="13"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>83</v>
+      <c r="A29" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>77</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>8</v>
@@ -1328,8 +1411,8 @@
       <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="28"/>
-      <c r="B30" s="22"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="20"/>
       <c r="C30" s="8" t="s">
         <v>21</v>
       </c>
@@ -1342,8 +1425,8 @@
       <c r="G30" s="9"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="28"/>
-      <c r="B31" s="22"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="20"/>
       <c r="C31" s="7" t="s">
         <v>24</v>
       </c>
@@ -1356,8 +1439,8 @@
       <c r="G31" s="9"/>
     </row>
     <row r="32" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="28"/>
-      <c r="B32" s="22"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="20"/>
       <c r="C32" s="8" t="s">
         <v>25</v>
       </c>
@@ -1370,40 +1453,40 @@
       <c r="G32" s="9"/>
     </row>
     <row r="33" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="28"/>
-      <c r="B33" s="22"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="20"/>
       <c r="C33" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D33" s="7">
         <v>1</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G33" s="9"/>
     </row>
     <row r="34" spans="1:7" ht="40" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="29"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F34" s="16"/>
-      <c r="G34" s="17"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" s="15"/>
+      <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" s="21" t="s">
-        <v>89</v>
+      <c r="A35" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>83</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>8</v>
@@ -1418,8 +1501,8 @@
       <c r="G35" s="6"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="19"/>
-      <c r="B36" s="22"/>
+      <c r="A36" s="18"/>
+      <c r="B36" s="20"/>
       <c r="C36" s="7" t="s">
         <v>21</v>
       </c>
@@ -1432,8 +1515,8 @@
       <c r="G36" s="9"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="19"/>
-      <c r="B37" s="22"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="7" t="s">
         <v>22</v>
       </c>
@@ -1446,8 +1529,8 @@
       <c r="G37" s="9"/>
     </row>
     <row r="38" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="19"/>
-      <c r="B38" s="22"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="20"/>
       <c r="C38" s="7" t="s">
         <v>13</v>
       </c>
@@ -1460,8 +1543,8 @@
       <c r="G38" s="9"/>
     </row>
     <row r="39" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="19"/>
-      <c r="B39" s="22"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="20"/>
       <c r="C39" s="7" t="s">
         <v>12</v>
       </c>
@@ -1474,10 +1557,10 @@
       <c r="G39" s="9"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="19"/>
-      <c r="B40" s="22"/>
+      <c r="A40" s="18"/>
+      <c r="B40" s="20"/>
       <c r="C40" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>9</v>
@@ -1488,11 +1571,11 @@
       <c r="G40" s="9"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="B41" s="21" t="s">
-        <v>86</v>
+      <c r="A41" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>80</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>8</v>
@@ -1507,8 +1590,8 @@
       <c r="G41" s="6"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="19"/>
-      <c r="B42" s="22"/>
+      <c r="A42" s="18"/>
+      <c r="B42" s="20"/>
       <c r="C42" s="7" t="s">
         <v>21</v>
       </c>
@@ -1521,8 +1604,8 @@
       <c r="G42" s="9"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="19"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="18"/>
+      <c r="B43" s="20"/>
       <c r="C43" s="7" t="s">
         <v>22</v>
       </c>
@@ -1535,8 +1618,8 @@
       <c r="G43" s="9"/>
     </row>
     <row r="44" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="19"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="20"/>
       <c r="C44" s="7" t="s">
         <v>13</v>
       </c>
@@ -1549,8 +1632,8 @@
       <c r="G44" s="9"/>
     </row>
     <row r="45" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="19"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="20"/>
       <c r="C45" s="7" t="s">
         <v>12</v>
       </c>
@@ -1563,10 +1646,10 @@
       <c r="G45" s="9"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="19"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="18"/>
+      <c r="B46" s="20"/>
       <c r="C46" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>9</v>
@@ -1577,8 +1660,8 @@
       <c r="G46" s="9"/>
     </row>
     <row r="47" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="19"/>
-      <c r="B47" s="22"/>
+      <c r="A47" s="18"/>
+      <c r="B47" s="20"/>
       <c r="C47" s="8" t="s">
         <v>15</v>
       </c>
@@ -1591,22 +1674,252 @@
       <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="20"/>
-      <c r="B48" s="23"/>
-      <c r="C48" s="15" t="s">
+      <c r="A48" s="18"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D48" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="15" t="s">
+      <c r="D48" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="F48" s="16"/>
-      <c r="G48" s="17"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="9"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="5"/>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="33"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="F50" s="28"/>
+      <c r="G50" s="9"/>
+    </row>
+    <row r="51" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="33"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F51" s="28"/>
+      <c r="G51" s="9"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="33"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E52" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="F52" s="28"/>
+      <c r="G52" s="9"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="33"/>
+      <c r="B53" s="31"/>
+      <c r="C53" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D53" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E53" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F53" s="28"/>
+      <c r="G53" s="9"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="33"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D54" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="F54" s="28"/>
+      <c r="G54" s="9"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="33"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E55" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F55" s="28"/>
+      <c r="G55" s="9"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="33"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D56" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="F56" s="28"/>
+      <c r="G56" s="9"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="33"/>
+      <c r="B57" s="31"/>
+      <c r="C57" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E57" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F57" s="28"/>
+      <c r="G57" s="9"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="33"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F58" s="28"/>
+      <c r="G58" s="9"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="33"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D59" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E59" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F59" s="28"/>
+      <c r="G59" s="9"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="33"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D60" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="E60" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F60" s="28"/>
+      <c r="G60" s="9"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="33"/>
+      <c r="B61" s="31"/>
+      <c r="C61" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D61" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E61" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="F61" s="28"/>
+      <c r="G61" s="9"/>
+    </row>
+    <row r="62" spans="1:7" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="33"/>
+      <c r="B62" s="31"/>
+      <c r="C62" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="D62" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E62" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="F62" s="28"/>
+      <c r="G62" s="9"/>
+    </row>
+    <row r="63" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="34"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F63" s="15"/>
+      <c r="G63" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B49:B63"/>
     <mergeCell ref="B41:B48"/>
     <mergeCell ref="B2:B28"/>
     <mergeCell ref="A2:A28"/>
@@ -1614,12 +1927,8 @@
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="B35:B40"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D13" r:id="rId1" xr:uid="{92E303BA-BCFD-48EF-8525-D40B11FD7176}"/>
-    <hyperlink ref="D21" r:id="rId2" display="zamansharmin000@gmail.com" xr:uid="{DB3C4841-5E61-4484-A613-DBF4C08C117C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1645,7 +1954,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1691,7 +2000,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1734,7 +2043,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1761,7 +2070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A088F9E1-D822-471E-B051-AB9AC78DDB3B}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -1777,7 +2086,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1820,7 +2129,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1847,7 +2156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A569904C-E53A-44CB-AA02-0DBE012274D9}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -1863,7 +2172,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>

</xml_diff>